<commit_message>
Re-run water chemistry analysis
</commit_message>
<xml_diff>
--- a/gp_review_2022/stations_used_2015.xlsx
+++ b/gp_review_2022/stations_used_2015.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Heleen_d_W\ICP_Waters\python_2020\icpw2\gp_review_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E81BA3-9821-45A5-9643-3A7354A14C87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA4E556-E7CC-4D73-95BB-09B4D745E770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{0DEDF1EC-9BA2-4CEF-9AEA-3FE174F6415A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0DEDF1EC-9BA2-4CEF-9AEA-3FE174F6415A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="168">
   <si>
     <t>Region</t>
   </si>
@@ -918,25 +918,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCCED8D-7DA0-4891-BDB4-65B980CB5A98}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:F1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.53125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.3984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -955,7 +955,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -972,7 +972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -989,7 +989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>Tr18_CZ01</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>Tr18_CZ02</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>Tr18_CZ03</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>Tr18_CZ04</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>Tr18_CZ05</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>Tr18_CZ06</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>Tr18_CZ07</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>Tr18_CZ08</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>DE02</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>DE07</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>DE08</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>DE10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>DE18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>DE21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>DE23</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>17</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>DE24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>DE27</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>DE28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>DE29</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>DE30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>DE33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>82</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>82</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>82</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>82</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>65</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>65</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>65</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>65</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>65</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>82</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>65</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>82</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>82</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>65</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>82</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>82</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>82</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>82</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>82</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>82</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>82</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>107</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>107</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>107</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>107</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>107</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>107</v>
       </c>
@@ -1914,7 +1914,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="B57" s="4"/>
       <c r="C57" s="5" t="s">
         <v>165</v>
@@ -1926,7 +1929,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>121</v>
       </c>
@@ -1944,7 +1947,7 @@
         <v>DE01</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>121</v>
       </c>
@@ -1962,7 +1965,7 @@
         <v>DE03</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>121</v>
       </c>
@@ -1980,7 +1983,7 @@
         <v>DE05</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>121</v>
       </c>
@@ -1998,7 +2001,7 @@
         <v>DE06</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>121</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>DE26</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>121</v>
       </c>

</xml_diff>